<commit_message>
Stromtarif-Programme vereinheitlicht EXCEL-Datei mit den aktuellen Stromtarifen
</commit_message>
<xml_diff>
--- a/SW/10_Aufgaben_mit_Funktionen_loesen/Stomtarif_Kosten.xlsx
+++ b/SW/10_Aufgaben_mit_Funktionen_loesen/Stomtarif_Kosten.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\Programmieren_lernen_2023\SW\10_Funktionen_konstruieren\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\Programmieren_lernen_2025\SW\10_Aufgaben_mit_Funktionen_loesen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326C790C-3E0A-4BB2-9B64-2C102C3C2DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE2F9A3-3964-4FAB-8CF3-D8DB36CE65D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{63FB9DFB-440C-492A-BA45-BA9DB5DE84BD}"/>
   </bookViews>
@@ -30,10 +30,10 @@
     <t>Verbrauch</t>
   </si>
   <si>
-    <t>Kosten2</t>
+    <t>Watt für wenig</t>
   </si>
   <si>
-    <t>Kosten1</t>
+    <t>Billig Strom</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Kosten1</c:v>
+                  <c:v>Watt für wenig</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -166,10 +166,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$16</c:f>
+              <c:f>Tabelle1!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -214,60 +214,66 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$16</c:f>
+              <c:f>Tabelle1!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>13.5</c:v>
+                  <c:v>15.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>18.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>25.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.5</c:v>
+                  <c:v>28.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>31.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58.5</c:v>
+                  <c:v>34.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>66</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>73.5</c:v>
+                  <c:v>41.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81</c:v>
+                  <c:v>44.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.5</c:v>
+                  <c:v>47.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96</c:v>
+                  <c:v>50.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>103.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>111</c:v>
+                  <c:v>57.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>118.5</c:v>
+                  <c:v>60.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>63.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -275,7 +281,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D2BB-4A71-9361-3FE0CF9D6FA1}"/>
+              <c16:uniqueId val="{00000000-FEE4-47B8-BF80-6264D7D8F2EF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -288,7 +294,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Kosten2</c:v>
+                  <c:v>Billig Strom</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -307,10 +313,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$16</c:f>
+              <c:f>Tabelle1!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -355,60 +361,66 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$16</c:f>
+              <c:f>Tabelle1!$C$2:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.3</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.400000000000002</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.5</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.600000000000009</c:v>
+                  <c:v>27.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.7</c:v>
+                  <c:v>30.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.8</c:v>
+                  <c:v>34.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>65.900000000000006</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74.000000000000014</c:v>
+                  <c:v>41.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>82.100000000000009</c:v>
+                  <c:v>45.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90.2</c:v>
+                  <c:v>48.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>98.300000000000011</c:v>
+                  <c:v>52.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>106.4</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>114.50000000000001</c:v>
+                  <c:v>59.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>122.60000000000001</c:v>
+                  <c:v>63.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>66.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -416,7 +428,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D2BB-4A71-9361-3FE0CF9D6FA1}"/>
+              <c16:uniqueId val="{00000001-FEE4-47B8-BF80-6264D7D8F2EF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -429,11 +441,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="547126072"/>
-        <c:axId val="547126776"/>
+        <c:axId val="455611032"/>
+        <c:axId val="455613848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="547126072"/>
+        <c:axId val="455611032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -476,7 +488,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="547126776"/>
+        <c:crossAx val="455613848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -484,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="547126776"/>
+        <c:axId val="455613848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +547,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="547126072"/>
+        <c:crossAx val="455611032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1175,23 +1187,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Diagramm 4">
+        <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{022C5ABA-036D-F0C1-E10C-A5280BB82D14}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C07AFAE6-4F35-676B-BE57-F5D7B9FB9AF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1509,23 +1521,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2B41E9-22BC-45A2-83E6-62CF2C2B41F4}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1533,12 +1548,12 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f xml:space="preserve"> 13.5 + A2 * 0.75</f>
-        <v>13.5</v>
+        <f xml:space="preserve"> 15.6 + A2 * 0.32</f>
+        <v>15.6</v>
       </c>
       <c r="C2">
-        <f xml:space="preserve"> 9.2 + A2 * 0.81</f>
-        <v>9.1999999999999993</v>
+        <f xml:space="preserve"> 12.8 + A2 * 0.36</f>
+        <v>12.8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1546,12 +1561,12 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B16" si="0" xml:space="preserve"> 13.5 + A3 * 0.75</f>
-        <v>21</v>
+        <f t="shared" ref="B3:B17" si="0" xml:space="preserve"> 15.6 + A3 * 0.32</f>
+        <v>18.8</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C16" si="1" xml:space="preserve"> 9.2 + A3 * 0.81</f>
-        <v>17.3</v>
+        <f t="shared" ref="C3:C17" si="1" xml:space="preserve"> 12.8 + A3 * 0.36</f>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1560,11 +1575,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>28.5</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>25.400000000000002</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1573,11 +1588,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>25.2</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>33.5</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1586,11 +1601,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>43.5</v>
+        <v>28.4</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>41.600000000000009</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1599,11 +1614,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>31.6</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>49.7</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1612,11 +1627,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>58.5</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>57.8</v>
+        <v>34.4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1625,11 +1640,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>65.900000000000006</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1638,11 +1653,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>73.5</v>
+        <v>41.2</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>74.000000000000014</v>
+        <v>41.599999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1651,11 +1666,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>44.4</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>82.100000000000009</v>
+        <v>45.2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1664,11 +1679,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>88.5</v>
+        <v>47.6</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>90.2</v>
+        <v>48.8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1677,11 +1692,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>50.800000000000004</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>98.300000000000011</v>
+        <v>52.400000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1690,11 +1705,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>103.5</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>106.4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1703,11 +1718,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>111</v>
+        <v>57.2</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>114.50000000000001</v>
+        <v>59.599999999999994</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1716,11 +1731,24 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>118.5</v>
+        <v>60.400000000000006</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>122.60000000000001</v>
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>63.6</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>66.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>